<commit_message>
first edition for LLG implementation
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/2_Short_Circuit_Results_PF_all.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/2_Short_Circuit_Results_PF_all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmaschke\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmaschke\PycharmProjects\pandapower\pandapower\test\shortcircuit\SCE_Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F079D4-CB30-4001-B914-9D7D371AA068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1947D-ABEA-420B-97FF-1D07949555EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-765" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{38FE6199-D0AE-4408-8F8D-48A6B774AFC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="7" activeTab="12" xr2:uid="{38FE6199-D0AE-4408-8F8D-48A6B774AFC7}"/>
   </bookViews>
   <sheets>
     <sheet name="3ph_max" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,16 @@
     <sheet name="2ph_min" sheetId="4" r:id="rId4"/>
     <sheet name="1ph_max" sheetId="5" r:id="rId5"/>
     <sheet name="1ph_min" sheetId="6" r:id="rId6"/>
+    <sheet name="3ph_max_fault" sheetId="7" r:id="rId7"/>
+    <sheet name="3ph_min_fault" sheetId="8" r:id="rId8"/>
+    <sheet name="2ph_max_fault" sheetId="9" r:id="rId9"/>
+    <sheet name="2ph_min_fault" sheetId="10" r:id="rId10"/>
+    <sheet name="1ph_max_fault" sheetId="11" r:id="rId11"/>
+    <sheet name="1ph_min_fault" sheetId="12" r:id="rId12"/>
+    <sheet name="LLG_max" sheetId="13" r:id="rId13"/>
+    <sheet name="LLG_min" sheetId="14" r:id="rId14"/>
+    <sheet name="LLG_max_fault" sheetId="15" r:id="rId15"/>
+    <sheet name="LLG_min_fault" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="26">
   <si>
     <t>Bus_0</t>
   </si>
@@ -174,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,11 +207,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -217,6 +242,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +601,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E3" sqref="E3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,10 +656,10 @@
         <v>100.000006</v>
       </c>
       <c r="E3" s="2">
-        <v>0.43781999999999999</v>
+        <v>0.43781639999999999</v>
       </c>
       <c r="F3" s="2">
-        <v>4.3781600000000003</v>
+        <v>4.3781635000000003</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -630,10 +676,10 @@
         <v>86.962535000000003</v>
       </c>
       <c r="E4" s="4">
-        <v>0.95782</v>
+        <v>0.95781640000000001</v>
       </c>
       <c r="F4" s="4">
-        <v>4.9681600000000001</v>
+        <v>4.9681635000000002</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -650,10 +696,10 @@
         <v>76.504824999999997</v>
       </c>
       <c r="E5" s="2">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="F5" s="2">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,10 +716,1935 @@
         <v>76.504824999999997</v>
       </c>
       <c r="E6" s="4">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="F6" s="4">
-        <v>5.55816</v>
+        <v>5.5581635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9F4266-CF54-44F1-853C-4AE925F5EBB3}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.241652</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.241652</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>14.337357000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>14.337357000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.50417429999999996</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5.0068970999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.111011</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.111011</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>12.828851</v>
+      </c>
+      <c r="H4" s="4">
+        <v>12.828851</v>
+      </c>
+      <c r="I4" s="4">
+        <v>7.6985422000000003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>6.4321967000000004</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.000723</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.000723</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>11.555358999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>11.555358999999999</v>
+      </c>
+      <c r="I5" s="2">
+        <v>14.821778399999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.8724382000000004</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.000723</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.000723</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>11.555358999999999</v>
+      </c>
+      <c r="H6" s="4">
+        <v>11.555358999999999</v>
+      </c>
+      <c r="I6" s="4">
+        <v>14.821778399999999</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.8724382000000004</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16B96AF-E600-4B00-A7CB-FD33A8F396FC}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.170817</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>13.51943</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.44288359999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.4027196999999996</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.0204690000000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>11.783358</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4.1859102999999998</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5.870495</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.90134099999999995</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>10.407794000000001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>7.8951758999999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.3350827000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5.5581635</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5.5581635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.90134099999999995</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10.407794000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>7.8951758999999999</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.3350827000000001</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="L6" s="4">
+        <v>5.5581635</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="N6" s="4">
+        <v>5.5581635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F553758-59DA-4F8B-AD1B-CE3E51F054E7}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.012886</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>11.695797000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.50417429999999996</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5.0068970999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.83519200000000005</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>9.6439690000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>7.6985422000000003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>6.4321967000000004</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.69991199999999998</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8.0818879999999993</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>14.821778399999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.8724382000000004</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.69991199999999998</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>8.0818879999999993</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>14.821778399999999</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.8724382000000004</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD3C6BB-D03B-4070-80AD-1A3C243A942A}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.884528</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.8835489999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>33.307656000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>33.296360999999997</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.44288450000000001</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.4027199000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.659694</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.0883820000000002</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>30.711503</v>
+      </c>
+      <c r="H4" s="4">
+        <v>24.114554999999999</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4.1853275999999999</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5.8711229999999999</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.3140830000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.728459</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>26.72073</v>
+      </c>
+      <c r="H5" s="2">
+        <v>19.95852</v>
+      </c>
+      <c r="I5" s="2">
+        <v>7.8945939000000003</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.335712</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5.5581635</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5.5581635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.3140830000000001</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.728459</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>26.72073</v>
+      </c>
+      <c r="H6" s="4">
+        <v>19.95852</v>
+      </c>
+      <c r="I6" s="4">
+        <v>7.8945939000000003</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.335712</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="L6" s="4">
+        <v>5.5581635</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="N6" s="4">
+        <v>5.5581635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96E11CF-3B57-4F5E-98C1-AD008F316AC2}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.3073950000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.306476</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>26.643498999999998</v>
+      </c>
+      <c r="H3" s="2">
+        <v>26.632895999999999</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.50417639999999997</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5.0068972</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.1446360000000002</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.5436209999999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>24.764126999999998</v>
+      </c>
+      <c r="H4" s="4">
+        <v>17.824204999999999</v>
+      </c>
+      <c r="I4" s="4">
+        <v>7.6974533000000003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>6.4348276999999996</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.791328</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.3123089999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>20.684477999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>15.153243</v>
+      </c>
+      <c r="I5" s="2">
+        <v>14.8206968</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.8750741</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.791328</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.3123089999999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>20.684477999999999</v>
+      </c>
+      <c r="H6" s="4">
+        <v>15.153243</v>
+      </c>
+      <c r="I6" s="4">
+        <v>14.8206968</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.8750741</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5CC6E8-3CC8-4897-943C-C43042DF166C}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.1709989999999999</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.1714929999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>13.521528999999999</v>
+      </c>
+      <c r="H3" s="2">
+        <v>13.527231</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.44288450000000001</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.4027199000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.1084799999999999</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.010054</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>12.799630000000001</v>
+      </c>
+      <c r="H4" s="4">
+        <v>11.663093999999999</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4.1853275999999999</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5.8711229999999999</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.040322</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.90168099999999995</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>12.012601999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10.411714</v>
+      </c>
+      <c r="I5" s="2">
+        <v>7.8945939000000003</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.335712</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5.5581635</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5.5581635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.040322</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.90168099999999995</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>12.012601999999999</v>
+      </c>
+      <c r="H6" s="4">
+        <v>10.411714</v>
+      </c>
+      <c r="I6" s="4">
+        <v>7.8945939000000003</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.335712</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="L6" s="4">
+        <v>5.5581635</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="N6" s="4">
+        <v>5.5581635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C02FFFE-90A8-4463-854B-D8EEFA1082BB}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.0131030000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.0135879999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>11.698305</v>
+      </c>
+      <c r="H3" s="2">
+        <v>11.70391</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.50417639999999997</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5.0068972</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.95757199999999998</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.81505700000000003</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>11.057084</v>
+      </c>
+      <c r="H4" s="4">
+        <v>9.4114730000000009</v>
+      </c>
+      <c r="I4" s="4">
+        <v>7.6974533000000003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>6.4348276999999996</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.87795199999999995</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.70994500000000005</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>10.13772</v>
+      </c>
+      <c r="H5" s="2">
+        <v>8.1977410000000006</v>
+      </c>
+      <c r="I5" s="2">
+        <v>14.8206968</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.8750741</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.87795199999999995</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.70994500000000005</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>10.13772</v>
+      </c>
+      <c r="H6" s="4">
+        <v>8.1977410000000006</v>
+      </c>
+      <c r="I6" s="4">
+        <v>14.8206968</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.8750741</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="L6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="N6" s="4">
+        <v>6.1551857999999999</v>
       </c>
     </row>
   </sheetData>
@@ -685,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2D4F11-E7D1-4631-B783-AE2DD2C13A43}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,10 +2712,10 @@
         <v>80.000003000000007</v>
       </c>
       <c r="E3" s="2">
-        <v>0.49752000000000002</v>
+        <v>0.49751859999999998</v>
       </c>
       <c r="F3" s="2">
-        <v>4.9751899999999996</v>
+        <v>4.9751858000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -761,10 +2732,10 @@
         <v>69.411537999999993</v>
       </c>
       <c r="E4" s="4">
-        <v>1.4959199999999999</v>
+        <v>1.4959186</v>
       </c>
       <c r="F4" s="4">
-        <v>5.5651900000000003</v>
+        <v>5.5651858000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,10 +2752,10 @@
         <v>60.228439999999999</v>
       </c>
       <c r="E5" s="2">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="F5" s="2">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -801,10 +2772,10 @@
         <v>60.228439999999999</v>
       </c>
       <c r="E6" s="4">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="F6" s="4">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
     </row>
   </sheetData>
@@ -814,273 +2785,369 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B856C-8A5C-4493-B232-1426670821F6}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I3" sqref="I3:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="I2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
         <v>2.5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="10">
         <v>2.5</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
         <v>28.867515000000001</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="10">
         <v>28.867515000000001</v>
       </c>
       <c r="I3" s="2">
-        <v>0.44288</v>
+        <v>0.44288359999999999</v>
       </c>
       <c r="J3" s="2">
-        <v>4.4027200000000004</v>
+        <v>4.4027196999999996</v>
       </c>
       <c r="K3" s="2">
-        <v>0.43781999999999999</v>
+        <v>0.43781639999999999</v>
       </c>
       <c r="L3" s="2">
-        <v>4.3781600000000003</v>
+        <v>4.3781635000000003</v>
       </c>
       <c r="M3" s="2">
-        <v>0.43781999999999999</v>
+        <v>0.43781639999999999</v>
       </c>
       <c r="N3" s="2">
-        <v>4.3781600000000003</v>
+        <v>4.3781635000000003</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
         <v>2.1740629999999999</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="12">
         <v>2.1740629999999999</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12">
         <v>25.103921</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="12">
         <v>25.103921</v>
       </c>
       <c r="I4" s="4">
-        <v>4.1859099999999998</v>
+        <v>4.1859102999999998</v>
       </c>
       <c r="J4" s="4">
-        <v>5.8704999999999998</v>
+        <v>5.870495</v>
       </c>
       <c r="K4" s="4">
-        <v>0.95782</v>
+        <v>0.95781640000000001</v>
       </c>
       <c r="L4" s="4">
-        <v>4.9681600000000001</v>
+        <v>4.9681635000000002</v>
       </c>
       <c r="M4" s="4">
-        <v>0.95782</v>
+        <v>0.95781640000000001</v>
       </c>
       <c r="N4" s="4">
-        <v>4.9681600000000001</v>
+        <v>4.9681635000000002</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
         <v>1.9126209999999999</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="10">
         <v>1.9126209999999999</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
         <v>22.085041</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="10">
         <v>22.085041</v>
       </c>
       <c r="I5" s="2">
-        <v>7.8951799999999999</v>
+        <v>7.8951758999999999</v>
       </c>
       <c r="J5" s="2">
-        <v>7.3350799999999996</v>
+        <v>7.3350827000000001</v>
       </c>
       <c r="K5" s="2">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="L5" s="2">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
       <c r="M5" s="2">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="N5" s="2">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
         <v>1.9126209999999999</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="12">
         <v>1.9126209999999999</v>
       </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="F6" s="12">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
         <v>22.085041</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="12">
         <v>22.085041</v>
       </c>
       <c r="I6" s="4">
-        <v>7.8951799999999999</v>
+        <v>7.8951758999999999</v>
       </c>
       <c r="J6" s="4">
-        <v>7.3350799999999996</v>
+        <v>7.3350827000000001</v>
       </c>
       <c r="K6" s="4">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="L6" s="4">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
       <c r="M6" s="4">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="N6" s="4">
-        <v>5.55816</v>
-      </c>
+        <v>5.5581635</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1092,7 +3159,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,22 +3274,22 @@
         <v>23.094011999999999</v>
       </c>
       <c r="I3" s="2">
-        <v>0.50417000000000001</v>
+        <v>0.50417429999999996</v>
       </c>
       <c r="J3" s="2">
-        <v>5.0068999999999999</v>
+        <v>5.0068970999999998</v>
       </c>
       <c r="K3" s="2">
-        <v>0.49752000000000002</v>
+        <v>0.49751859999999998</v>
       </c>
       <c r="L3" s="2">
-        <v>4.9751899999999996</v>
+        <v>4.9751858000000002</v>
       </c>
       <c r="M3" s="2">
-        <v>0.49752000000000002</v>
+        <v>0.49751859999999998</v>
       </c>
       <c r="N3" s="2">
-        <v>4.9751899999999996</v>
+        <v>4.9751858000000002</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1251,22 +3318,22 @@
         <v>20.037385</v>
       </c>
       <c r="I4" s="4">
-        <v>7.6985400000000004</v>
+        <v>7.6985422000000003</v>
       </c>
       <c r="J4" s="4">
-        <v>6.4321999999999999</v>
+        <v>6.4321967000000004</v>
       </c>
       <c r="K4" s="4">
-        <v>1.4959199999999999</v>
+        <v>1.4959186</v>
       </c>
       <c r="L4" s="4">
-        <v>5.5651900000000003</v>
+        <v>5.5651858000000001</v>
       </c>
       <c r="M4" s="4">
-        <v>1.4959199999999999</v>
+        <v>1.4959186</v>
       </c>
       <c r="N4" s="4">
-        <v>5.5651900000000003</v>
+        <v>5.5651858000000001</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1295,22 +3362,22 @@
         <v>17.386452999999999</v>
       </c>
       <c r="I5" s="2">
-        <v>14.82178</v>
+        <v>14.821778399999999</v>
       </c>
       <c r="J5" s="2">
-        <v>7.8724400000000001</v>
+        <v>7.8724382000000004</v>
       </c>
       <c r="K5" s="2">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="L5" s="2">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
       <c r="M5" s="2">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="N5" s="2">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1339,22 +3406,22 @@
         <v>17.386452999999999</v>
       </c>
       <c r="I6" s="4">
-        <v>14.82178</v>
+        <v>14.821778399999999</v>
       </c>
       <c r="J6" s="4">
-        <v>7.8724400000000001</v>
+        <v>7.8724382000000004</v>
       </c>
       <c r="K6" s="4">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="L6" s="4">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
       <c r="M6" s="4">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="N6" s="4">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1367,7 +3434,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,22 +3549,22 @@
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>0.44288</v>
+        <v>0.44288359999999999</v>
       </c>
       <c r="J3" s="2">
-        <v>4.4027200000000004</v>
+        <v>4.4027196999999996</v>
       </c>
       <c r="K3" s="2">
-        <v>0.43781999999999999</v>
+        <v>0.43781639999999999</v>
       </c>
       <c r="L3" s="2">
-        <v>4.3781600000000003</v>
+        <v>4.3781635000000003</v>
       </c>
       <c r="M3" s="2">
-        <v>0.43781999999999999</v>
+        <v>0.43781639999999999</v>
       </c>
       <c r="N3" s="2">
-        <v>4.3781600000000003</v>
+        <v>4.3781635000000003</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1526,22 +3593,22 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>4.1859099999999998</v>
+        <v>4.1859102999999998</v>
       </c>
       <c r="J4" s="4">
-        <v>5.8704999999999998</v>
+        <v>5.870495</v>
       </c>
       <c r="K4" s="4">
-        <v>0.95782</v>
+        <v>0.95781640000000001</v>
       </c>
       <c r="L4" s="4">
-        <v>4.9681600000000001</v>
+        <v>4.9681635000000002</v>
       </c>
       <c r="M4" s="4">
-        <v>0.95782</v>
+        <v>0.95781640000000001</v>
       </c>
       <c r="N4" s="4">
-        <v>4.9681600000000001</v>
+        <v>4.9681635000000002</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1570,22 +3637,22 @@
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>7.8951799999999999</v>
+        <v>7.8951758999999999</v>
       </c>
       <c r="J5" s="2">
-        <v>7.3350799999999996</v>
+        <v>7.3350827000000001</v>
       </c>
       <c r="K5" s="2">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="L5" s="2">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
       <c r="M5" s="2">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="N5" s="2">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1614,22 +3681,22 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>7.8951799999999999</v>
+        <v>7.8951758999999999</v>
       </c>
       <c r="J6" s="4">
-        <v>7.3350799999999996</v>
+        <v>7.3350827000000001</v>
       </c>
       <c r="K6" s="4">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="L6" s="4">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
       <c r="M6" s="4">
-        <v>1.4778199999999999</v>
+        <v>1.4778164</v>
       </c>
       <c r="N6" s="4">
-        <v>5.55816</v>
+        <v>5.5581635</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +3709,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,22 +3824,22 @@
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>0.50417000000000001</v>
+        <v>0.50417429999999996</v>
       </c>
       <c r="J3" s="2">
-        <v>5.0068999999999999</v>
+        <v>5.0068970999999998</v>
       </c>
       <c r="K3" s="2">
-        <v>0.49752000000000002</v>
+        <v>0.49751859999999998</v>
       </c>
       <c r="L3" s="2">
-        <v>4.9751899999999996</v>
+        <v>4.9751858000000002</v>
       </c>
       <c r="M3" s="2">
-        <v>0.49752000000000002</v>
+        <v>0.49751859999999998</v>
       </c>
       <c r="N3" s="2">
-        <v>4.9751899999999996</v>
+        <v>4.9751858000000002</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1801,22 +3868,22 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>7.6985400000000004</v>
+        <v>7.6985422000000003</v>
       </c>
       <c r="J4" s="4">
-        <v>6.4321999999999999</v>
+        <v>6.4321967000000004</v>
       </c>
       <c r="K4" s="4">
-        <v>1.4959199999999999</v>
+        <v>1.4959186</v>
       </c>
       <c r="L4" s="4">
-        <v>5.5651900000000003</v>
+        <v>5.5651858000000001</v>
       </c>
       <c r="M4" s="4">
-        <v>1.4959199999999999</v>
+        <v>1.4959186</v>
       </c>
       <c r="N4" s="4">
-        <v>5.5651900000000003</v>
+        <v>5.5651858000000001</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1845,22 +3912,22 @@
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>14.82178</v>
+        <v>14.821778399999999</v>
       </c>
       <c r="J5" s="2">
-        <v>7.8724400000000001</v>
+        <v>7.8724382000000004</v>
       </c>
       <c r="K5" s="2">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="L5" s="2">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
       <c r="M5" s="2">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="N5" s="2">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1889,23 +3956,616 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>14.82178</v>
+        <v>14.821778399999999</v>
       </c>
       <c r="J6" s="4">
-        <v>7.8724400000000001</v>
+        <v>7.8724382000000004</v>
       </c>
       <c r="K6" s="4">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="L6" s="4">
-        <v>6.1551900000000002</v>
+        <v>6.1551857999999999</v>
       </c>
       <c r="M6" s="4">
-        <v>2.4943200000000001</v>
+        <v>2.4943186000000002</v>
       </c>
       <c r="N6" s="4">
-        <v>6.1551900000000002</v>
-      </c>
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E97624C-0E61-4B77-AE32-6D04B4DB3B07}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.171673</v>
+      </c>
+      <c r="D3" s="2">
+        <v>40.587955000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.0937570000000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>37.888841999999997</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.025409</v>
+      </c>
+      <c r="D5" s="2">
+        <v>35.521210000000004</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5.5581635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.025409</v>
+      </c>
+      <c r="D6" s="4">
+        <v>35.521210000000004</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.5581635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6135C5F1-7230-4D1B-9722-4C965775F0AC}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.0138039999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>35.119210000000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.49751859999999998</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.9751858000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.93102799999999997</v>
+      </c>
+      <c r="D4" s="4">
+        <v>32.251761000000002</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.4959186</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5.5651858000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.85922500000000002</v>
+      </c>
+      <c r="D5" s="2">
+        <v>29.764427000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="F5" s="2">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.85922500000000002</v>
+      </c>
+      <c r="D6" s="4">
+        <v>29.764427000000001</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.4943186000000002</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6.1551857999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3E6B89-937B-45D9-B66A-34769CBA8785}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.470726</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.470726</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>16.982485</v>
+      </c>
+      <c r="H3" s="2">
+        <v>16.982485</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.44288359999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.4027196999999996</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.43781639999999999</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4.3781635000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.336603</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.336603</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>15.433757</v>
+      </c>
+      <c r="H4" s="4">
+        <v>15.433757</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4.1859102999999998</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5.870495</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.95781640000000001</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4.9681635000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.2240599999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.2240599999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>14.134221999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>14.134221999999999</v>
+      </c>
+      <c r="I5" s="2">
+        <v>7.8951758999999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.3350827000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5.5581635</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.4778164</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5.5581635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.2240599999999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.2240599999999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>14.134221999999999</v>
+      </c>
+      <c r="H6" s="4">
+        <v>14.134221999999999</v>
+      </c>
+      <c r="I6" s="4">
+        <v>7.8951758999999999</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.3350827000000001</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="L6" s="4">
+        <v>5.5581635</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.4778164</v>
+      </c>
+      <c r="N6" s="4">
+        <v>5.5581635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
renaming 3,2,1 ph to lll, ll, lg
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/2_Short_Circuit_Results_PF_all.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/2_Short_Circuit_Results_PF_all.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmaschke\PycharmProjects\pandapower\pandapower\test\shortcircuit\SCE_Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1947D-ABEA-420B-97FF-1D07949555EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89C802B-ACDD-4777-B290-5577E6C27369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="7" activeTab="12" xr2:uid="{38FE6199-D0AE-4408-8F8D-48A6B774AFC7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{38FE6199-D0AE-4408-8F8D-48A6B774AFC7}"/>
   </bookViews>
   <sheets>
-    <sheet name="3ph_max" sheetId="1" r:id="rId1"/>
-    <sheet name="3ph_min" sheetId="2" r:id="rId2"/>
-    <sheet name="2ph_max" sheetId="3" r:id="rId3"/>
-    <sheet name="2ph_min" sheetId="4" r:id="rId4"/>
-    <sheet name="1ph_max" sheetId="5" r:id="rId5"/>
-    <sheet name="1ph_min" sheetId="6" r:id="rId6"/>
-    <sheet name="3ph_max_fault" sheetId="7" r:id="rId7"/>
-    <sheet name="3ph_min_fault" sheetId="8" r:id="rId8"/>
-    <sheet name="2ph_max_fault" sheetId="9" r:id="rId9"/>
-    <sheet name="2ph_min_fault" sheetId="10" r:id="rId10"/>
-    <sheet name="1ph_max_fault" sheetId="11" r:id="rId11"/>
-    <sheet name="1ph_min_fault" sheetId="12" r:id="rId12"/>
+    <sheet name="LLL_max" sheetId="1" r:id="rId1"/>
+    <sheet name="LLL_min" sheetId="2" r:id="rId2"/>
+    <sheet name="LL_max" sheetId="3" r:id="rId3"/>
+    <sheet name="LL_min" sheetId="4" r:id="rId4"/>
+    <sheet name="LG_max" sheetId="5" r:id="rId5"/>
+    <sheet name="LG_min" sheetId="6" r:id="rId6"/>
+    <sheet name="LLL_max_fault" sheetId="7" r:id="rId7"/>
+    <sheet name="LLL_min_fault" sheetId="8" r:id="rId8"/>
+    <sheet name="LL_max_fault" sheetId="9" r:id="rId9"/>
+    <sheet name="LL_min_fault" sheetId="10" r:id="rId10"/>
+    <sheet name="LG_max_fault" sheetId="11" r:id="rId11"/>
+    <sheet name="LG_min_fault" sheetId="12" r:id="rId12"/>
     <sheet name="LLG_max" sheetId="13" r:id="rId13"/>
     <sheet name="LLG_min" sheetId="14" r:id="rId14"/>
     <sheet name="LLG_max_fault" sheetId="15" r:id="rId15"/>
@@ -226,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -264,6 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1282,7 +1283,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD3C6BB-D03B-4070-80AD-1A3C243A942A}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,6 +1822,9 @@
       <c r="N6" s="4">
         <v>5.5581635</v>
       </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2106,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5CC6E8-3CC8-4897-943C-C43042DF166C}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,7 +2386,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N6"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3709,7 +3713,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="F1" sqref="F1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4245,8 +4249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3E6B89-937B-45D9-B66A-34769CBA8785}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>